<commit_message>
ptit commit avant de tester méthode de treshold
</commit_message>
<xml_diff>
--- a/00 - Documentation/Etat_art/tableau_recap_etat_art.xlsx
+++ b/00 - Documentation/Etat_art/tableau_recap_etat_art.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
   <si>
     <t>Article</t>
   </si>
@@ -107,6 +107,52 @@
   <si>
     <t>"Scatter matrix"
 "Shrinkage Method"</t>
+  </si>
+  <si>
+    <t>The classification of skateboarding tricks via Transfer learning pipelines</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Reconnaissance de figures de skate en utilisant des </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>transfer pipelines.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+  </si>
+  <si>
+    <t>Utilisation des données accélérométriques gyroscopiques (MPU6050) 
+Figures testées : Ollie;Kickflip, shoveit, Nollie, fs 180
+Feature &lt;=&gt; images ici -&gt; c'est le role des tranferts pipelines qui extraiait des fetaures 
+Utilisation des 6 données brut et de leur CWT 
+Optimized SVM, avec différents kernek et autres hyper paramètre
+Très bon résultats</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SVM
+CWT = plus pratique que fft askip
+</t>
+  </si>
+  <si>
+    <t>CWT
+Transfer pipelines</t>
   </si>
 </sst>
 </file>
@@ -174,11 +220,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -462,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="B5" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -479,11 +525,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -508,7 +554,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="5" customFormat="1" ht="144" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -531,7 +577,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" s="5" customFormat="1" ht="222.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" s="4" customFormat="1" ht="222.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>14</v>
       </c>
@@ -552,7 +598,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" s="4" customFormat="1" ht="273" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>18</v>
       </c>
@@ -573,14 +619,26 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
+    <row r="6" spans="1:7" s="4" customFormat="1" ht="275.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="3">
+        <v>2021</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2"/>

</xml_diff>